<commit_message>
Primeras 30 imagenes en monitorizar
</commit_message>
<xml_diff>
--- a/data/info_especies.xlsx
+++ b/data/info_especies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efa949d9f75320b2/Documentos/_Salinas/proyecto_especies/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_FFC65FC07BF1ECFCD2170B473B7EDCD86582C291" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80F72126-BB4C-4D23-8779-ECA6BC70EF61}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_FFC65FC07BF1ECFCD2170B473B7EDCD86582C291" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{369134EE-C4C4-447F-B221-846553798372}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -716,11 +716,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>